<commit_message>
hvdc generator in progress
</commit_message>
<xml_diff>
--- a/data/case9.xlsx
+++ b/data/case9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46109FC2-8E23-4491-B799-723267B2802F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B64D8D-950D-4944-8049-0B5515CC9A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hvdc" sheetId="12" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="118">
   <si>
     <t>name</t>
   </si>
@@ -381,16 +381,10 @@
     <t>D3</t>
   </si>
   <si>
-    <t>continuous_output</t>
-  </si>
-  <si>
-    <t>short_output</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>HVDC</t>
   </si>
 </sst>
 </file>
@@ -465,7 +459,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -782,46 +776,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F936777E-A678-467D-AA50-B7F1A2F38BF3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>2400</v>
+      </c>
+      <c r="I2">
         <v>2200</v>
       </c>
-      <c r="D2">
-        <v>2400</v>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -830,7 +877,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:Y4"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,12 +955,8 @@
       <c r="W1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1130,7 +1173,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1183,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1229,7 +1272,7 @@
         <v>27</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -1572,17 +1615,6 @@
       </c>
       <c r="L10">
         <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="K11">
-        <v>1000</v>
-      </c>
-      <c r="L11">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1628,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,7 +1723,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A11" sqref="A11:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2111,7 +2143,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
hvdc international as gen with prices + unlimited power eu side
</commit_message>
<xml_diff>
--- a/data/case9.xlsx
+++ b/data/case9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74164A56-2429-42EA-A430-BFBD96715557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5110581-DFE3-46BB-88AF-FD5CE024B6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33480" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hvdc" sheetId="12" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="228">
   <si>
     <t>name</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Ireland_HVDC</t>
   </si>
   <si>
-    <t>N. Ireland_HVDC</t>
-  </si>
-  <si>
     <t>D4</t>
   </si>
   <si>
@@ -725,6 +722,12 @@
   </si>
   <si>
     <t>Western_Link</t>
+  </si>
+  <si>
+    <t>marginal_cost</t>
+  </si>
+  <si>
+    <t>N_Ireland_HVDC</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -817,11 +820,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -832,6 +844,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1148,15 +1163,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F936777E-A678-467D-AA50-B7F1A2F38BF3}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1199,10 +1214,13 @@
       <c r="N1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1243,10 +1261,13 @@
       <c r="N2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3">
         <v>29</v>
@@ -1287,8 +1308,11 @@
       <c r="N3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1331,8 +1355,11 @@
       <c r="N4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1375,8 +1402,11 @@
       <c r="N5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -1419,8 +1449,11 @@
       <c r="N6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1463,10 +1496,13 @@
       <c r="N7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>227</v>
       </c>
       <c r="B8">
         <v>34</v>
@@ -1506,6 +1542,9 @@
       </c>
       <c r="N8" t="s">
         <v>60</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1518,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1605,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1673,7 +1712,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1741,7 +1780,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1809,7 +1848,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1877,7 +1916,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1945,7 +1984,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2013,7 +2052,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2081,7 +2120,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2149,7 +2188,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2217,7 +2256,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2285,7 +2324,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2353,7 +2392,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2421,7 +2460,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2489,7 +2528,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2557,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2625,7 +2664,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2693,7 +2732,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2761,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2829,7 +2868,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2897,7 +2936,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2965,7 +3004,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3033,7 +3072,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3101,7 +3140,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3169,7 +3208,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3237,7 +3276,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3305,7 +3344,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3373,7 +3412,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3441,7 +3480,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -5235,7 +5274,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -5256,7 +5295,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -5277,7 +5316,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -5298,7 +5337,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -5319,7 +5358,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -5340,7 +5379,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -5361,7 +5400,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -5382,7 +5421,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -5403,7 +5442,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -5424,7 +5463,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -5445,7 +5484,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <v>13</v>
@@ -5466,7 +5505,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -5487,7 +5526,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -5508,7 +5547,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -5529,7 +5568,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>17</v>
@@ -5550,7 +5589,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -5571,7 +5610,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21">
         <v>19</v>
@@ -5592,7 +5631,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -5613,7 +5652,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23">
         <v>21</v>
@@ -5634,7 +5673,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24">
         <v>22</v>
@@ -5655,7 +5694,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25">
         <v>23</v>
@@ -5676,7 +5715,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -5697,7 +5736,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27">
         <v>25</v>
@@ -5718,7 +5757,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28">
         <v>26</v>
@@ -5739,7 +5778,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29">
         <v>27</v>
@@ -5760,7 +5799,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30">
         <v>28</v>
@@ -5841,7 +5880,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5882,7 +5921,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5923,7 +5962,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5964,7 +6003,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -6005,7 +6044,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -6046,7 +6085,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6087,7 +6126,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -6128,7 +6167,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -6169,7 +6208,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -6210,7 +6249,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -6251,7 +6290,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -6292,7 +6331,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -6333,7 +6372,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -6374,7 +6413,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -6415,7 +6454,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -6456,7 +6495,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -6497,7 +6536,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -6538,7 +6577,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -6579,7 +6618,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -6620,7 +6659,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -6661,7 +6700,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -6702,7 +6741,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -6743,7 +6782,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -6784,7 +6823,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -6825,7 +6864,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -6866,7 +6905,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -6907,7 +6946,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -6948,7 +6987,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -6989,7 +7028,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -7030,7 +7069,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31">
         <v>9</v>
@@ -7071,7 +7110,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32">
         <v>9</v>
@@ -7112,7 +7151,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -7153,7 +7192,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -7194,7 +7233,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35">
         <v>10</v>
@@ -7235,7 +7274,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36">
         <v>10</v>
@@ -7276,7 +7315,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -7317,7 +7356,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38">
         <v>10</v>
@@ -7358,7 +7397,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B39">
         <v>11</v>
@@ -7399,7 +7438,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40">
         <v>11</v>
@@ -7440,7 +7479,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41">
         <v>11</v>
@@ -7481,7 +7520,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42">
         <v>11</v>
@@ -7522,7 +7561,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43">
         <v>12</v>
@@ -7563,7 +7602,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44">
         <v>12</v>
@@ -7604,7 +7643,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B45">
         <v>12</v>
@@ -7645,7 +7684,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46">
         <v>12</v>
@@ -7686,7 +7725,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47">
         <v>12</v>
@@ -7727,7 +7766,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B48">
         <v>12</v>
@@ -7768,7 +7807,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B49">
         <v>13</v>
@@ -7809,7 +7848,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B50">
         <v>13</v>
@@ -7850,7 +7889,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B51">
         <v>14</v>
@@ -7891,7 +7930,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B52">
         <v>14</v>
@@ -7932,7 +7971,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B53">
         <v>14</v>
@@ -7973,7 +8012,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54">
         <v>14</v>
@@ -8014,7 +8053,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B55">
         <v>15</v>
@@ -8055,7 +8094,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B56">
         <v>15</v>
@@ -8096,7 +8135,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57">
         <v>16</v>
@@ -8137,7 +8176,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58">
         <v>16</v>
@@ -8178,7 +8217,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59">
         <v>16</v>
@@ -8219,7 +8258,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B60">
         <v>16</v>
@@ -8260,7 +8299,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61">
         <v>17</v>
@@ -8301,7 +8340,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B62">
         <v>17</v>
@@ -8342,7 +8381,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63">
         <v>17</v>
@@ -8383,7 +8422,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B64">
         <v>17</v>
@@ -8424,7 +8463,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65">
         <v>19</v>
@@ -8465,7 +8504,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B66">
         <v>19</v>
@@ -8506,7 +8545,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B67">
         <v>19</v>
@@ -8547,7 +8586,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68">
         <v>19</v>
@@ -8588,7 +8627,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B69">
         <v>20</v>
@@ -8629,7 +8668,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B70">
         <v>20</v>
@@ -8670,7 +8709,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71">
         <v>20</v>
@@ -8711,7 +8750,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B72">
         <v>20</v>
@@ -8752,7 +8791,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73">
         <v>20</v>
@@ -8793,7 +8832,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B74">
         <v>20</v>
@@ -8834,7 +8873,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75">
         <v>20</v>
@@ -8875,7 +8914,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B76">
         <v>20</v>
@@ -8916,7 +8955,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77">
         <v>21</v>
@@ -8957,7 +8996,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78">
         <v>21</v>
@@ -8998,7 +9037,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79">
         <v>21</v>
@@ -9039,7 +9078,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80">
         <v>21</v>
@@ -9080,7 +9119,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81">
         <v>21</v>
@@ -9121,7 +9160,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B82">
         <v>21</v>
@@ -9162,7 +9201,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B83">
         <v>22</v>
@@ -9203,7 +9242,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84">
         <v>22</v>
@@ -9244,7 +9283,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85">
         <v>22</v>
@@ -9285,7 +9324,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B86">
         <v>22</v>
@@ -9326,7 +9365,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B87">
         <v>22</v>
@@ -9367,7 +9406,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B88">
         <v>22</v>
@@ -9408,7 +9447,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B89">
         <v>23</v>
@@ -9449,7 +9488,7 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B90">
         <v>23</v>
@@ -9490,7 +9529,7 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91">
         <v>23</v>
@@ -9531,7 +9570,7 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B92">
         <v>23</v>
@@ -9572,7 +9611,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93">
         <v>24</v>
@@ -9613,7 +9652,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B94">
         <v>24</v>
@@ -9654,7 +9693,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B95">
         <v>26</v>
@@ -9695,7 +9734,7 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B96">
         <v>26</v>
@@ -9736,7 +9775,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B97">
         <v>27</v>
@@ -9777,7 +9816,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B98">
         <v>27</v>
@@ -9818,7 +9857,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B99">
         <v>28</v>
@@ -9859,7 +9898,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B100">
         <v>28</v>
@@ -9900,7 +9939,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B101">
         <v>29</v>
@@ -9941,7 +9980,7 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B102">
         <v>33</v>
@@ -9982,7 +10021,7 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B103">
         <v>34</v>
@@ -10023,7 +10062,7 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B104">
         <v>30</v>
@@ -10064,7 +10103,7 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B105">
         <v>31</v>
@@ -10105,7 +10144,7 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B106">
         <v>32</v>

</xml_diff>